<commit_message>
stats & report adjustment
</commit_message>
<xml_diff>
--- a/reports/templates/daily.xlsx
+++ b/reports/templates/daily.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uicestone/Sites/kangazone-server/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0191283A-58E6-2642-A2C0-6F9D490B5BA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEDCB6D-1BF4-3147-A99F-1DB523D6279F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20640" windowHeight="17540" tabRatio="180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,10 +154,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{{creditAmount}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{{socksAmount}}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -210,10 +206,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{{creditAmountM}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{{restaurantAmountM}}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -255,6 +247,14 @@
   </si>
   <si>
     <t>{{bookingAmountM}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{creditAndCodeAmount}}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{creditAndCodeAmountM}}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -718,7 +718,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -769,10 +769,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20" customHeight="1">
@@ -783,7 +783,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="20" customHeight="1">
@@ -794,7 +794,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="20" customHeight="1">
@@ -805,7 +805,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="20" customHeight="1">
@@ -813,10 +813,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="20" customHeight="1">
@@ -824,10 +824,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="20" customHeight="1">
@@ -835,10 +835,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20" customHeight="1">
@@ -846,10 +846,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="20" customHeight="1">
@@ -857,7 +857,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="5"/>
     </row>
@@ -889,10 +889,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="20" customHeight="1">
@@ -900,10 +900,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="20" customHeight="1">
@@ -911,10 +911,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="20" customHeight="1">
@@ -922,10 +922,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="20" customHeight="1">
@@ -933,10 +933,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="20" customHeight="1">
@@ -963,10 +963,10 @@
         <v>21</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="20" customHeight="1">

</xml_diff>